<commit_message>
Changed captured pieces save logic.
</commit_message>
<xml_diff>
--- a/Doc/JSDraughts.xlsx
+++ b/Doc/JSDraughts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
   <si>
     <t>A</t>
   </si>
@@ -60,6 +60,9 @@
   </si>
   <si>
     <t>Original Board with numbers</t>
+  </si>
+  <si>
+    <t>Capure index</t>
   </si>
 </sst>
 </file>
@@ -531,15 +534,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="S15" sqref="S15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="8" width="3.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="3" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
     <col min="12" max="19" width="3.21875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3" bestFit="1" customWidth="1"/>
   </cols>
@@ -930,6 +934,18 @@
       <c r="H12" s="20"/>
       <c r="I12" s="20"/>
       <c r="J12" s="20"/>
+      <c r="K12" s="20" t="s">
+        <v>12</v>
+      </c>
+      <c r="L12" s="20"/>
+      <c r="M12" s="20"/>
+      <c r="N12" s="20"/>
+      <c r="O12" s="20"/>
+      <c r="P12" s="20"/>
+      <c r="Q12" s="20"/>
+      <c r="R12" s="20"/>
+      <c r="S12" s="20"/>
+      <c r="T12" s="20"/>
     </row>
     <row r="13" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
@@ -955,6 +971,26 @@
       </c>
       <c r="I13" t="s">
         <v>7</v>
+      </c>
+      <c r="K13" s="8"/>
+      <c r="L13" s="8">
+        <v>47</v>
+      </c>
+      <c r="M13" s="8"/>
+      <c r="N13" s="8">
+        <v>47</v>
+      </c>
+      <c r="O13" s="8"/>
+      <c r="P13" s="8">
+        <v>47</v>
+      </c>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="8">
+        <v>47</v>
+      </c>
+      <c r="S13" s="8"/>
+      <c r="T13" s="8">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:20" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
@@ -972,6 +1008,24 @@
       <c r="J14">
         <v>8</v>
       </c>
+      <c r="K14" s="8"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="10">
+        <v>47</v>
+      </c>
+      <c r="N14" s="2"/>
+      <c r="O14" s="10">
+        <v>47</v>
+      </c>
+      <c r="P14" s="2"/>
+      <c r="Q14" s="10">
+        <v>47</v>
+      </c>
+      <c r="R14" s="2"/>
+      <c r="S14" s="14">
+        <v>47</v>
+      </c>
+      <c r="T14" s="8"/>
     </row>
     <row r="15" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15">
@@ -988,6 +1042,26 @@
       <c r="J15">
         <v>7</v>
       </c>
+      <c r="K15" s="8"/>
+      <c r="L15" s="9">
+        <v>47</v>
+      </c>
+      <c r="M15" s="4"/>
+      <c r="N15" s="12">
+        <v>15</v>
+      </c>
+      <c r="O15" s="4"/>
+      <c r="P15" s="12">
+        <v>16</v>
+      </c>
+      <c r="Q15" s="4"/>
+      <c r="R15" s="12">
+        <v>17</v>
+      </c>
+      <c r="S15" s="5"/>
+      <c r="T15" s="8">
+        <v>47</v>
+      </c>
     </row>
     <row r="16" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16">
@@ -1004,8 +1078,26 @@
       <c r="J16">
         <v>6</v>
       </c>
-    </row>
-    <row r="17" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K16" s="8"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="12">
+        <v>12</v>
+      </c>
+      <c r="N16" s="4"/>
+      <c r="O16" s="12">
+        <v>13</v>
+      </c>
+      <c r="P16" s="4"/>
+      <c r="Q16" s="12">
+        <v>14</v>
+      </c>
+      <c r="R16" s="4"/>
+      <c r="S16" s="15">
+        <v>47</v>
+      </c>
+      <c r="T16" s="8"/>
+    </row>
+    <row r="17" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1020,8 +1112,28 @@
       <c r="J17">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K17" s="8"/>
+      <c r="L17" s="9">
+        <v>47</v>
+      </c>
+      <c r="M17" s="4"/>
+      <c r="N17" s="12">
+        <v>9</v>
+      </c>
+      <c r="O17" s="4"/>
+      <c r="P17" s="12">
+        <v>10</v>
+      </c>
+      <c r="Q17" s="4"/>
+      <c r="R17" s="12">
+        <v>11</v>
+      </c>
+      <c r="S17" s="5"/>
+      <c r="T17" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1036,8 +1148,26 @@
       <c r="J18">
         <v>4</v>
       </c>
-    </row>
-    <row r="19" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K18" s="8"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="12">
+        <v>6</v>
+      </c>
+      <c r="N18" s="4"/>
+      <c r="O18" s="12">
+        <v>7</v>
+      </c>
+      <c r="P18" s="4"/>
+      <c r="Q18" s="12">
+        <v>8</v>
+      </c>
+      <c r="R18" s="4"/>
+      <c r="S18" s="15">
+        <v>47</v>
+      </c>
+      <c r="T18" s="8"/>
+    </row>
+    <row r="19" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1052,8 +1182,28 @@
       <c r="J19">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="K19" s="8"/>
+      <c r="L19" s="9">
+        <v>47</v>
+      </c>
+      <c r="M19" s="4"/>
+      <c r="N19" s="12">
+        <v>3</v>
+      </c>
+      <c r="O19" s="4"/>
+      <c r="P19" s="12">
+        <v>4</v>
+      </c>
+      <c r="Q19" s="4"/>
+      <c r="R19" s="12">
+        <v>5</v>
+      </c>
+      <c r="S19" s="5"/>
+      <c r="T19" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1068,8 +1218,26 @@
       <c r="J20">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="K20" s="8"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="12">
+        <v>0</v>
+      </c>
+      <c r="N20" s="4"/>
+      <c r="O20" s="12">
+        <v>1</v>
+      </c>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="12">
+        <v>2</v>
+      </c>
+      <c r="R20" s="4"/>
+      <c r="S20" s="15">
+        <v>47</v>
+      </c>
+      <c r="T20" s="8"/>
+    </row>
+    <row r="21" spans="1:20" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1084,8 +1252,28 @@
       <c r="J21">
         <v>1</v>
       </c>
-    </row>
-    <row r="22" spans="1:10" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="K21" s="8"/>
+      <c r="L21" s="11">
+        <v>47</v>
+      </c>
+      <c r="M21" s="6"/>
+      <c r="N21" s="13">
+        <v>47</v>
+      </c>
+      <c r="O21" s="6"/>
+      <c r="P21" s="13">
+        <v>47</v>
+      </c>
+      <c r="Q21" s="6"/>
+      <c r="R21" s="13">
+        <v>47</v>
+      </c>
+      <c r="S21" s="7"/>
+      <c r="T21" s="8">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1110,8 +1298,28 @@
       <c r="I22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K22" s="8">
+        <v>47</v>
+      </c>
+      <c r="L22" s="8"/>
+      <c r="M22" s="8">
+        <v>47</v>
+      </c>
+      <c r="N22" s="8"/>
+      <c r="O22" s="8">
+        <v>47</v>
+      </c>
+      <c r="P22" s="8"/>
+      <c r="Q22" s="8">
+        <v>47</v>
+      </c>
+      <c r="R22" s="8"/>
+      <c r="S22" s="8">
+        <v>47</v>
+      </c>
+      <c r="T22" s="8"/>
+    </row>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>11</v>
       </c>
@@ -1125,7 +1333,7 @@
       <c r="I24" s="20"/>
       <c r="J24" s="20"/>
     </row>
-    <row r="25" spans="1:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -1151,7 +1359,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="26" spans="1:10" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1175,7 +1383,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1199,7 +1407,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -1223,7 +1431,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -1247,7 +1455,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
@@ -1271,7 +1479,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -1295,7 +1503,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>
@@ -1370,11 +1578,12 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="5">
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="K1:T1"/>
     <mergeCell ref="A12:J12"/>
     <mergeCell ref="A24:J24"/>
+    <mergeCell ref="K12:T12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Testing capture  move or take back error
</commit_message>
<xml_diff>
--- a/Doc/JSDraughts.xlsx
+++ b/Doc/JSDraughts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="15">
   <si>
     <t>A</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>Capure index</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>o</t>
   </si>
 </sst>
 </file>
@@ -103,7 +109,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -125,6 +131,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFCCECFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -221,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -247,6 +259,7 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -532,10 +545,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z34"/>
+  <dimension ref="A1:AI34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3"/>
+      <selection activeCell="AG5" sqref="AG5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -546,9 +559,10 @@
     <col min="11" max="11" width="3" bestFit="1" customWidth="1"/>
     <col min="12" max="19" width="3.21875" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="3" bestFit="1" customWidth="1"/>
+    <col min="28" max="35" width="3.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>8</v>
       </c>
@@ -573,7 +587,7 @@
       <c r="S1" s="20"/>
       <c r="T1" s="20"/>
     </row>
-    <row r="2" spans="1:26" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:35" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="10">
         <v>28</v>
@@ -612,7 +626,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:26" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:35" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9">
         <v>24</v>
       </c>
@@ -662,8 +676,20 @@
         <f>X3=Y3</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AC3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG3" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AI3" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="3"/>
       <c r="B4" s="12">
         <v>20</v>
@@ -715,8 +741,18 @@
         <f t="shared" ref="Z4:Z34" si="1">X4=Y4</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AB4" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AD4" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF4" s="21"/>
+      <c r="AH4" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="9">
         <v>16</v>
       </c>
@@ -766,8 +802,18 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="6" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AC5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AE5" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="AG5" s="21"/>
+      <c r="AI5" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="6" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="3"/>
       <c r="B6" s="12">
         <v>12</v>
@@ -819,8 +865,14 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AB6" s="21"/>
+      <c r="AD6" s="21"/>
+      <c r="AF6" s="21"/>
+      <c r="AH6" s="21" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="9">
         <v>8</v>
       </c>
@@ -870,8 +922,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="8" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AC7" s="21"/>
+      <c r="AE7" s="21"/>
+      <c r="AG7" s="21"/>
+      <c r="AI7" s="21"/>
+    </row>
+    <row r="8" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
       <c r="B8" s="12">
         <v>4</v>
@@ -923,8 +979,18 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:26" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AB8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF8" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH8" s="21"/>
+    </row>
+    <row r="9" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="11">
         <v>0</v>
       </c>
@@ -974,8 +1040,20 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:26" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="AC9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AE9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG9" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AI9" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:35" ht="16.8" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="K10" s="8"/>
       <c r="L10" s="11">
         <v>5</v>
@@ -1010,8 +1088,20 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-    </row>
-    <row r="11" spans="1:26" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AB10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AD10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF10" s="21" t="s">
+        <v>14</v>
+      </c>
+      <c r="AH10" s="21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="K11" s="8">
         <v>0</v>
       </c>
@@ -1047,7 +1137,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.3">
       <c r="A12" s="20" t="s">
         <v>10</v>
       </c>
@@ -1087,7 +1177,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>0</v>
       </c>
@@ -1147,7 +1237,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:26" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:35" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>8</v>
       </c>
@@ -1195,7 +1285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1245,7 +1335,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:26" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>6</v>
       </c>

</xml_diff>

<commit_message>
Fixed situation, when no moves left.
</commit_message>
<xml_diff>
--- a/Doc/JSDraughts.xlsx
+++ b/Doc/JSDraughts.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="16">
   <si>
     <t>A</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>o</t>
+  </si>
+  <si>
+    <t>Move: x</t>
   </si>
 </sst>
 </file>
@@ -545,10 +548,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AI34"/>
+  <dimension ref="A1:AJ34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AB32" sqref="AB32"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="AJ31" sqref="AJ31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1425,7 +1428,7 @@
       <c r="AF16" s="19"/>
       <c r="AH16" s="19"/>
     </row>
-    <row r="17" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>5</v>
       </c>
@@ -1483,7 +1486,7 @@
       </c>
       <c r="AI17" s="19"/>
     </row>
-    <row r="18" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>4</v>
       </c>
@@ -1539,7 +1542,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="19" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>3</v>
       </c>
@@ -1601,7 +1604,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="20" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>2</v>
       </c>
@@ -1659,7 +1662,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:35" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:36" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>1</v>
       </c>
@@ -1709,7 +1712,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:35" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:36" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B22" t="s">
         <v>0</v>
       </c>
@@ -1769,7 +1772,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:36" x14ac:dyDescent="0.3">
       <c r="W23">
         <v>28</v>
       </c>
@@ -1784,20 +1787,12 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AC23" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AE23" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AG23" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AI23" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="24" spans="1:35" x14ac:dyDescent="0.3">
+      <c r="AC23" s="19"/>
+      <c r="AE23" s="19"/>
+      <c r="AG23" s="19"/>
+      <c r="AI23" s="19"/>
+    </row>
+    <row r="24" spans="1:36" x14ac:dyDescent="0.3">
       <c r="A24" s="21" t="s">
         <v>11</v>
       </c>
@@ -1824,20 +1819,14 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AB24" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AD24" s="19" t="s">
-        <v>13</v>
-      </c>
-      <c r="AF24" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="AB24" s="19"/>
+      <c r="AD24" s="19"/>
+      <c r="AF24" s="19"/>
       <c r="AH24" s="19" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="25" spans="1:35" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:36" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>0</v>
       </c>
@@ -1881,11 +1870,9 @@
         <v>13</v>
       </c>
       <c r="AG25" s="19"/>
-      <c r="AI25" s="19" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="26" spans="1:35" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AI25" s="19"/>
+    </row>
+    <row r="26" spans="1:36" ht="16.2" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>8</v>
       </c>
@@ -1923,13 +1910,11 @@
         <v>1</v>
       </c>
       <c r="AB26" s="19"/>
-      <c r="AD26" s="19" t="s">
-        <v>13</v>
-      </c>
+      <c r="AD26" s="19"/>
       <c r="AF26" s="19"/>
       <c r="AH26" s="19"/>
     </row>
-    <row r="27" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>7</v>
       </c>
@@ -1967,13 +1952,15 @@
         <v>1</v>
       </c>
       <c r="AC27" s="19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="AE27" s="19"/>
       <c r="AG27" s="19"/>
-      <c r="AI27" s="19"/>
-    </row>
-    <row r="28" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AI27" s="19" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>6</v>
       </c>
@@ -2011,15 +1998,11 @@
         <v>1</v>
       </c>
       <c r="AB28" s="19"/>
-      <c r="AD28" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="AD28" s="19"/>
       <c r="AF28" s="19"/>
-      <c r="AH28" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="29" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AH28" s="19"/>
+    </row>
+    <row r="29" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>5</v>
       </c>
@@ -2065,11 +2048,9 @@
       <c r="AG29" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="AI29" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="30" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AI29" s="19"/>
+    </row>
+    <row r="30" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2106,18 +2087,15 @@
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="AB30" s="19" t="s">
-        <v>14</v>
-      </c>
+      <c r="AB30" s="19"/>
       <c r="AD30" s="19"/>
-      <c r="AF30" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="AH30" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="31" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="AF30" s="19"/>
+      <c r="AH30" s="19"/>
+      <c r="AJ30" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="31" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>3</v>
       </c>
@@ -2155,7 +2133,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:35" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:36" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>2</v>
       </c>

</xml_diff>